<commit_message>
man_slice log msg modification
</commit_message>
<xml_diff>
--- a/raw_data/res.xlsx
+++ b/raw_data/res.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">mean</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">angle3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size3</t>
   </si>
   <si>
     <t xml:space="preserve">cell4</t>
@@ -155,16 +158,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AT15"/>
+  <dimension ref="A1:AT16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
@@ -441,47 +441,39 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>0.096</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>0.162</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>0.068</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>0.051</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>0.099</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>0.082</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <f aca="false">AVERAGE(B11:K11)</f>
-        <v>0.0783</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <f aca="false">STDEV(B11:K11)</f>
-        <v>0.0356901791658278</v>
+      <c r="B10" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>230</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,77 +481,77 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.162</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <f aca="false">AVERAGE(B12:K12)</f>
+        <v>0.0783</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <f aca="false">STDEV(B12:K12)</f>
+        <v>0.0356901791658278</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C13" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F13" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G13" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I13" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J13" s="0" t="n">
         <v>160</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K13" s="0" t="n">
         <v>175</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>0.151</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0.236</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>0.136</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0.186</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>0.131</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>0.166</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>0.082</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>0.122</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>0.104</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <f aca="false">AVERAGE(B14:K14)</f>
-        <v>0.1594</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <f aca="false">STDEV(B14:K14)</f>
-        <v>0.0605955627271686</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,33 +559,76 @@
         <v>12</v>
       </c>
       <c r="B15" s="0" t="n">
+        <v>0.151</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.236</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0.166</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">AVERAGE(B15:K15)</f>
+        <v>0.1594</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <f aca="false">STDEV(B15:K15)</f>
+        <v>0.0605955627271686</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C16" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D16" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F16" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G16" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H16" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I16" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J16" s="0" t="n">
         <v>160</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K16" s="0" t="n">
         <v>170</v>
       </c>
     </row>

</xml_diff>